<commit_message>
work on task 3
</commit_message>
<xml_diff>
--- a/ResultsTask3/Task3_Analysis.xlsx
+++ b/ResultsTask3/Task3_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fnoardo/Documents/geoBIM/benchmark/benchmarkExe/FinalOutcomes/ResultsTask3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D091A42-DB20-724A-8E13-6B66BEC33745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81EA38E-CE71-0045-A136-DE401B87565F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29100" yWindow="460" windowWidth="38100" windowHeight="21140" xr2:uid="{840C6D61-1AE8-634C-990F-82DFAF05BE31}"/>
+    <workbookView xWindow="28940" yWindow="460" windowWidth="38100" windowHeight="21140" xr2:uid="{840C6D61-1AE8-634C-990F-82DFAF05BE31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6135" uniqueCount="1269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6149" uniqueCount="1276">
   <si>
     <t>#</t>
   </si>
@@ -3970,12 +3970,33 @@
     <t>The software uses a relational database for data storage. Oracle, PostGreSQL and MS SQL Server
 are supported by the software. Oracle was used in the benchmark Task 3 experiment.</t>
   </si>
+  <si>
+    <t>Dean Hintz</t>
+  </si>
+  <si>
+    <t>dean.hintz@safe.com</t>
+  </si>
+  <si>
+    <t>FME 2019.2</t>
+  </si>
+  <si>
+    <t>Spatial ETL</t>
+  </si>
+  <si>
+    <t>No special configuration is necessary to achieve ADE support other than to specify the path or paths to the ADE application schema within the ‘Additional ADE schema files’ reader or writer setting. ADE’s are fully supported on both reader and writing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have provided comprehensive CityGML support for more than a decade, so offer perhaps some of the most extensive support in the industry. We also provide citygml importers and exporters to many software vendors such as AutoDesk, ESRI and others. </t>
+  </si>
+  <si>
+    <t>Yes. Not sure what is meant by ‘native format’. CityGML is OGC GML with the CityGML standard group of application schemas. We support CityGML v0.4, 1.0, 2.0 and have done extensive testing with the draft CityGML v3.0 schemas, although in the latter case we used our generic GML reader / writer which is more flexible since v3.0 is still in development.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4017,6 +4038,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF3C4257"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -4045,7 +4087,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4067,6 +4109,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4448,13 +4496,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9A080F-CA6B-8D40-BDA5-3EED01E2D04C}">
-  <dimension ref="A1:Y420"/>
+  <dimension ref="A1:AM420"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="U381" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="U6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="X407" sqref="X407"/>
+      <selection pane="bottomRight" activeCell="AA27" sqref="AA27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4464,7 +4512,7 @@
     <col min="24" max="25" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4529,7 +4577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -4599,8 +4647,11 @@
       <c r="Y2" s="8" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA2" s="16" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>38</v>
       </c>
@@ -4670,8 +4721,11 @@
       <c r="Y3" s="9" t="s">
         <v>1211</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="AA3" s="13" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>56</v>
       </c>
@@ -4741,8 +4795,11 @@
       <c r="Y4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>62</v>
       </c>
@@ -4812,8 +4869,11 @@
       <c r="Y5" s="8" t="s">
         <v>1213</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA5" s="17" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>79</v>
       </c>
@@ -4883,8 +4943,11 @@
       <c r="Y6" s="8" t="s">
         <v>1214</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>95</v>
       </c>
@@ -4954,8 +5017,11 @@
       <c r="Y7" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>98</v>
       </c>
@@ -5026,7 +5092,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>116</v>
       </c>
@@ -5090,8 +5156,11 @@
       <c r="U9" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA9" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>120</v>
       </c>
@@ -5159,7 +5228,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>122</v>
       </c>
@@ -5230,7 +5299,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>140</v>
       </c>
@@ -5301,7 +5370,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>156</v>
       </c>
@@ -5372,7 +5441,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>173</v>
       </c>
@@ -5443,7 +5512,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>190</v>
       </c>
@@ -5514,7 +5583,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>203</v>
       </c>
@@ -5585,7 +5654,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>220</v>
       </c>
@@ -5656,7 +5725,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>236</v>
       </c>
@@ -5726,8 +5795,11 @@
       <c r="Y18" s="8" t="s">
         <v>1226</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="AA18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>240</v>
       </c>
@@ -5797,8 +5869,11 @@
       <c r="Y19" s="8" t="s">
         <v>1226</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" ht="68" x14ac:dyDescent="0.2">
+      <c r="AA19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>242</v>
       </c>
@@ -5862,8 +5937,11 @@
       <c r="U20" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA20" s="18" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>249</v>
       </c>
@@ -5876,7 +5954,7 @@
         <v>https://api.typeform.com/responses/files/0b7bd8a26aee39e8ae750f2acbe5bdc830f15aaba6eceb1224bcc16651709494/FZKViewer51_ADEsDirectory.jpg</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>250</v>
       </c>
@@ -5946,8 +6024,11 @@
       <c r="Y22" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>251</v>
       </c>
@@ -6017,8 +6098,11 @@
       <c r="Y23" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="AA23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>252</v>
       </c>
@@ -6082,8 +6166,11 @@
       <c r="U24" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>120</v>
       </c>
@@ -6148,7 +6235,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>253</v>
       </c>
@@ -6218,8 +6305,11 @@
       <c r="Y26" t="s">
         <v>1218</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="AA26" s="16" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>261</v>
       </c>
@@ -6289,8 +6379,11 @@
       <c r="Y27" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA27" s="16" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>120</v>
       </c>
@@ -6355,7 +6448,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>263</v>
       </c>
@@ -6420,7 +6513,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>120</v>
       </c>
@@ -6485,7 +6578,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>267</v>
       </c>
@@ -6550,7 +6643,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>269</v>
       </c>
@@ -22413,7 +22506,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="385" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:39" ht="34" x14ac:dyDescent="0.2">
       <c r="A385" s="11" t="s">
         <v>1146</v>
       </c>
@@ -22466,7 +22559,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="386" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A386" s="11" t="s">
         <v>120</v>
       </c>
@@ -22516,7 +22609,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="387" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:39" ht="34" x14ac:dyDescent="0.2">
       <c r="A387" s="11" t="s">
         <v>1147</v>
       </c>
@@ -22565,8 +22658,9 @@
       <c r="U387" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="388" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="AM387" s="15"/>
+    </row>
+    <row r="388" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A388" s="11" t="s">
         <v>120</v>
       </c>
@@ -22616,7 +22710,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="389" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A389" s="11" t="s">
         <v>1148</v>
       </c>
@@ -22666,7 +22760,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="390" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:39" ht="34" x14ac:dyDescent="0.2">
       <c r="A390" s="11" t="s">
         <v>687</v>
       </c>
@@ -22719,7 +22813,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="391" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:39" ht="34" x14ac:dyDescent="0.2">
       <c r="A391" s="11" t="s">
         <v>1150</v>
       </c>
@@ -22772,7 +22866,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="392" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A392" s="11" t="s">
         <v>120</v>
       </c>
@@ -22822,7 +22916,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="393" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:39" ht="34" x14ac:dyDescent="0.2">
       <c r="A393" s="11" t="s">
         <v>1151</v>
       </c>
@@ -22872,7 +22966,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="394" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A394" s="11" t="s">
         <v>1152</v>
       </c>
@@ -22880,7 +22974,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="395" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A395" s="11" t="s">
         <v>1153</v>
       </c>
@@ -22930,7 +23024,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="396" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:39" ht="34" x14ac:dyDescent="0.2">
       <c r="A396" s="11" t="s">
         <v>1155</v>
       </c>
@@ -22983,7 +23077,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="397" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A397" s="11" t="s">
         <v>120</v>
       </c>
@@ -23033,7 +23127,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="398" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A398" s="11" t="s">
         <v>705</v>
       </c>
@@ -23083,7 +23177,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="399" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A399" s="11" t="s">
         <v>1157</v>
       </c>
@@ -23133,7 +23227,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="400" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A400" s="11" t="s">
         <v>1158</v>
       </c>
@@ -24150,8 +24244,9 @@
     <hyperlink ref="X384" r:id="rId22" xr:uid="{BCDAC7F8-BDF9-3749-B223-DFF8E73B4649}"/>
     <hyperlink ref="Y384" r:id="rId23" xr:uid="{29461078-89B5-9349-A830-AEFE0616A1EF}"/>
     <hyperlink ref="X394" r:id="rId24" xr:uid="{B99B9CDF-E4C3-004D-AE95-1442165A4B84}"/>
+    <hyperlink ref="AA3" r:id="rId25" display="mailto:dean.hintz@safe.com" xr:uid="{1CFC2911-FF1F-7940-86CF-FE3C14BB1709}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId25"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>